<commit_message>
add missing key resources and rerun
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="951">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2853,6 +2853,21 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/bash/run-gistic.sh ; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/bash/run_gistic_consensus.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnnotSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/annotsv.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FusionAnnotator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/fusion_annotator.cwl</t>
   </si>
 </sst>
 </file>
@@ -7867,6 +7882,39 @@
         <v>945</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>946</v>
+      </c>
+      <c r="B22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>947</v>
+      </c>
+      <c r="B23" t="s">
+        <v>636</v>
+      </c>
+      <c r="C23" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>949</v>
+      </c>
+      <c r="B24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
response to @sjspielman code review
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="949">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2847,12 +2847,6 @@
   </si>
   <si>
     <t xml:space="preserve">bcftools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GISTIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/bash/run-gistic.sh ; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/bash/run_gistic_consensus.sh</t>
   </si>
   <si>
     <t xml:space="preserve">RSEM</t>
@@ -7876,21 +7870,21 @@
         <v>944</v>
       </c>
       <c r="B21" t="s">
-        <v>901</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s">
-        <v>945</v>
+        <v>919</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>945</v>
+      </c>
+      <c r="B22" t="s">
+        <v>636</v>
+      </c>
+      <c r="C22" t="s">
         <v>946</v>
-      </c>
-      <c r="B22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="23">
@@ -7898,21 +7892,10 @@
         <v>947</v>
       </c>
       <c r="B23" t="s">
-        <v>636</v>
+        <v>482</v>
       </c>
       <c r="C23" t="s">
         <v>948</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>949</v>
-      </c>
-      <c r="B24" t="s">
-        <v>482</v>
-      </c>
-      <c r="C24" t="s">
-        <v>950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating GATK, RNASeQC, minor update to Table 2 based on clinician conversations
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="959">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2804,12 +2804,27 @@
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-cram-only-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-fq-input.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-fq-input-cram-only-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mendqc-wf.cwl</t>
   </si>
   <si>
-    <t xml:space="preserve">GATK</t>
+    <t xml:space="preserve">GATK (alignment)</t>
   </si>
   <si>
     <t xml:space="preserve">4.0.3.0</t>
   </si>
   <si>
+    <t xml:space="preserve">GATK (single sample genotyping)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0.12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-single-genotype-basic.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATK (VariantFiltration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.8.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">lancet</t>
   </si>
   <si>
@@ -2822,12 +2837,6 @@
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mendqc-wf.cwl</t>
   </si>
   <si>
-    <t xml:space="preserve">4.0.12.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mutect2_strelka2-wf.cwl</t>
-  </si>
-  <si>
     <t xml:space="preserve">VarDict Java</t>
   </si>
   <si>
@@ -2852,6 +2861,12 @@
     <t xml:space="preserve">RSEM</t>
   </si>
   <si>
+    <t xml:space="preserve">RNA-SeQC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">AnnotSV</t>
   </si>
   <si>
@@ -2870,25 +2885,13 @@
     <t xml:space="preserve">4.3t</t>
   </si>
   <si>
-    <t xml:space="preserve">https://sourceforge.net/projects/snpeff/files/snpEff_v4_3t_core.zip</t>
+    <t xml:space="preserve">FILL IN</t>
   </si>
   <si>
     <t xml:space="preserve">ANNOVAR</t>
   </si>
   <si>
-    <t xml:space="preserve">2020Jun08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://annovar.openbioinformatics.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InterVar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/WGLab/InterVar/blob/4801682d37982bb3e99b50392790878a568b42cd/Intervar.py</t>
+    <t xml:space="preserve">20190319</t>
   </si>
 </sst>
 </file>
@@ -7831,40 +7834,40 @@
         <v>931</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>932</v>
       </c>
       <c r="C15" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>934</v>
+      </c>
+      <c r="B16" t="s">
+        <v>935</v>
+      </c>
+      <c r="C16" t="s">
         <v>933</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="B17" t="s">
-        <v>935</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B18" t="s">
-        <v>938</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>939</v>
@@ -7886,51 +7889,51 @@
         <v>943</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>944</v>
       </c>
       <c r="C20" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>919</v>
+        <v>945</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B22" t="s">
-        <v>636</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>946</v>
+        <v>919</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B23" t="s">
-        <v>482</v>
+        <v>949</v>
       </c>
       <c r="C23" t="s">
-        <v>948</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B24" t="s">
-        <v>950</v>
+        <v>636</v>
       </c>
       <c r="C24" t="s">
         <v>951</v>
@@ -7941,21 +7944,32 @@
         <v>952</v>
       </c>
       <c r="B25" t="s">
+        <v>482</v>
+      </c>
+      <c r="C25" t="s">
         <v>953</v>
-      </c>
-      <c r="C25" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>954</v>
+      </c>
+      <c r="B26" t="s">
         <v>955</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>956</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>957</v>
+      </c>
+      <c r="B27" t="s">
+        <v>958</v>
+      </c>
+      <c r="C27" t="s">
+        <v>956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add germline variants, ANNOVAR/SNPeff code link
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="960">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2885,13 +2885,16 @@
     <t xml:space="preserve">4.3t</t>
   </si>
   <si>
-    <t xml:space="preserve">FILL IN</t>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/clinvar_pathogenic_filter.cwl</t>
   </si>
   <si>
     <t xml:space="preserve">ANNOVAR</t>
   </si>
   <si>
-    <t xml:space="preserve">20190319</t>
+    <t xml:space="preserve">2018-04-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/annovar_20190319.cwl</t>
   </si>
 </sst>
 </file>
@@ -7969,7 +7972,7 @@
         <v>958</v>
       </c>
       <c r="C27" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add germline tools to KR table/update table 2 (#1577)
* add germline tools

* updating GATK, RNASeQC, minor update to Table 2 based on clinician conversations

* update annovar version

* add germline variants, ANNOVAR/SNPeff code link

* add additional tools

* revert RNA-SeQC to 2.3.4
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="966">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2780,6 +2780,12 @@
     <t xml:space="preserve">rsem</t>
   </si>
   <si>
+    <t xml:space="preserve">Cutadapt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">STAR-Fusion</t>
   </si>
   <si>
@@ -2804,12 +2810,27 @@
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-cram-only-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-fq-input.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-fq-input-cram-only-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-alignment-wf.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mendqc-wf.cwl</t>
   </si>
   <si>
-    <t xml:space="preserve">GATK</t>
+    <t xml:space="preserve">GATK (alignment)</t>
   </si>
   <si>
     <t xml:space="preserve">4.0.3.0</t>
   </si>
   <si>
+    <t xml:space="preserve">GATK (single sample genotyping)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0.12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-single-genotype-basic.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATK (VariantFiltration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.8.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">lancet</t>
   </si>
   <si>
@@ -2822,13 +2843,7 @@
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mendqc-wf.cwl</t>
   </si>
   <si>
-    <t xml:space="preserve">4.0.12.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mutect2_strelka2-wf.cwl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VarDict Java v1.5.8</t>
+    <t xml:space="preserve">VarDict Java</t>
   </si>
   <si>
     <t xml:space="preserve">1.5.8</t>
@@ -2846,12 +2861,24 @@
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc_annot_vcf_sub_wf.cwl</t>
   </si>
   <si>
+    <t xml:space="preserve">VCFtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1.15</t>
+  </si>
+  <si>
     <t xml:space="preserve">bcftools</t>
   </si>
   <si>
     <t xml:space="preserve">RSEM</t>
   </si>
   <si>
+    <t xml:space="preserve">RNA-SeQC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">AnnotSV</t>
   </si>
   <si>
@@ -2862,6 +2889,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/fusion_annotator.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNPeff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.3t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/clinvar_pathogenic_filter.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANNOVAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-04-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/annovar_20190319.cwl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picard Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.18.2-SNAPSHOT</t>
   </si>
 </sst>
 </file>
@@ -7749,7 +7800,7 @@
         <v>921</v>
       </c>
       <c r="B10" t="s">
-        <v>867</v>
+        <v>922</v>
       </c>
       <c r="C10" t="s">
         <v>919</v>
@@ -7757,10 +7808,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>867</v>
       </c>
       <c r="C11" t="s">
         <v>919</v>
@@ -7768,35 +7819,35 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B12" t="s">
-        <v>924</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>925</v>
+        <v>919</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>925</v>
+      </c>
+      <c r="B13" t="s">
         <v>926</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>927</v>
-      </c>
-      <c r="C13" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>928</v>
+      </c>
+      <c r="B14" t="s">
         <v>929</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>930</v>
-      </c>
-      <c r="C14" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="15">
@@ -7804,10 +7855,10 @@
         <v>931</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>932</v>
       </c>
       <c r="C15" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
     </row>
     <row r="16">
@@ -7815,29 +7866,29 @@
         <v>933</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>934</v>
       </c>
       <c r="C16" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>929</v>
+        <v>936</v>
       </c>
       <c r="B17" t="s">
+        <v>937</v>
+      </c>
+      <c r="C17" t="s">
         <v>935</v>
-      </c>
-      <c r="C17" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B18" t="s">
-        <v>938</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>939</v>
@@ -7848,54 +7899,131 @@
         <v>940</v>
       </c>
       <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
         <v>941</v>
-      </c>
-      <c r="C19" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>942</v>
+      </c>
+      <c r="B20" t="s">
         <v>943</v>
       </c>
-      <c r="B20" t="s">
-        <v>115</v>
-      </c>
       <c r="C20" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>946</v>
       </c>
       <c r="C21" t="s">
-        <v>919</v>
+        <v>947</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="B22" t="s">
-        <v>636</v>
+        <v>949</v>
       </c>
       <c r="C22" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>950</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
         <v>947</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>951</v>
+      </c>
+      <c r="B24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>952</v>
+      </c>
+      <c r="B25" t="s">
+        <v>953</v>
+      </c>
+      <c r="C25" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>954</v>
+      </c>
+      <c r="B26" t="s">
+        <v>636</v>
+      </c>
+      <c r="C26" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>956</v>
+      </c>
+      <c r="B27" t="s">
         <v>482</v>
       </c>
-      <c r="C23" t="s">
-        <v>948</v>
+      <c r="C27" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>958</v>
+      </c>
+      <c r="B28" t="s">
+        <v>959</v>
+      </c>
+      <c r="C28" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>961</v>
+      </c>
+      <c r="B29" t="s">
+        <v>962</v>
+      </c>
+      <c r="C29" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>964</v>
+      </c>
+      <c r="B30" t="s">
+        <v>965</v>
+      </c>
+      <c r="C30" t="s">
+        <v>930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Table 1 to include patient-level Ns
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="958">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -134,6 +134,12 @@
     <t xml:space="preserve">1.0.7</t>
   </si>
   <si>
+    <t xml:space="preserve">berryFunctions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.18.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BH</t>
   </si>
   <si>
@@ -413,12 +419,6 @@
     <t xml:space="preserve">0.8.5</t>
   </si>
   <si>
-    <t xml:space="preserve">d3treeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">data.table</t>
   </si>
   <si>
@@ -782,342 +782,321 @@
     <t xml:space="preserve">1.34.0</t>
   </si>
   <si>
-    <t xml:space="preserve">ggfittext</t>
+    <t xml:space="preserve">ggforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggfortify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggplot2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggpubr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggrepel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggsci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggsignif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggthemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggupset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1.0.9000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git2r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmnetUtils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalOptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmailr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5-13.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gplots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridExtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridGraphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSEABase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hexbin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.27.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4.7.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hmisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmlTable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.13.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmltools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmlwidgets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">httpuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">httr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hunspell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hwriter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">igraph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immunedeconv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">influenceR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interactiveDisplayBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.24.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ipred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRanges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.20.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iterators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">janitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jsonlite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kknn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km.ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMsurv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knitr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lahman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">later</t>
   </si>
   <si>
     <t xml:space="preserve">0.8.0</t>
   </si>
   <si>
-    <t xml:space="preserve">ggforce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggfortify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggpattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggplot2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggpubr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggrepel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggsci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggsignif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggthemes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggupset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1.0.9000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git2r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glmnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glmnetUtils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalOptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmailr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5-13.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gplots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridBase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridExtra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridGeometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridGraphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridSVG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSEABase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gtable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gtools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hexbin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.27.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highlight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4.7.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hmisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmlTable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.13.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmltools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmlwidgets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">httpuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">httr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hunspell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hwriter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">igraph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">immunedeconv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">influenceR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interactiveDisplayBase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.24.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ipred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRanges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.20.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iterators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">janitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jsonlite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kknn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">km.ci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMsurv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">knitr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labeling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lahman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda.r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">later</t>
-  </si>
-  <si>
     <t xml:space="preserve">lattice</t>
   </si>
   <si>
@@ -1259,6 +1238,12 @@
     <t xml:space="preserve">0.7-25</t>
   </si>
   <si>
+    <t xml:space="preserve">mclust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.4.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">MCPcounter</t>
   </si>
   <si>
@@ -1310,6 +1295,12 @@
     <t xml:space="preserve">6.2.1</t>
   </si>
   <si>
+    <t xml:space="preserve">MultiAssayExperiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.10.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">multipanelfigure</t>
   </si>
   <si>
@@ -1424,12 +1415,6 @@
     <t xml:space="preserve">pingr</t>
   </si>
   <si>
-    <t xml:space="preserve">pipeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6.1.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">pkgbuild</t>
   </si>
   <si>
@@ -1574,6 +1559,9 @@
     <t xml:space="preserve">2.4.0</t>
   </si>
   <si>
+    <t xml:space="preserve">RaggedExperiment</t>
+  </si>
+  <si>
     <t xml:space="preserve">rappdirs</t>
   </si>
   <si>
@@ -1850,9 +1838,6 @@
     <t xml:space="preserve">0.7-5</t>
   </si>
   <si>
-    <t xml:space="preserve">shades</t>
-  </si>
-  <si>
     <t xml:space="preserve">shape</t>
   </si>
   <si>
@@ -1964,9 +1949,6 @@
     <t xml:space="preserve">1.16.1</t>
   </si>
   <si>
-    <t xml:space="preserve">sunburstR</t>
-  </si>
-  <si>
     <t xml:space="preserve">survival</t>
   </si>
   <si>
@@ -2040,12 +2022,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.4-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treemapify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5.2</t>
   </si>
   <si>
     <t xml:space="preserve">tweenr</t>
@@ -3529,15 +3505,15 @@
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
@@ -3569,31 +3545,31 @@
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45">
@@ -3657,15 +3633,15 @@
         <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54">
@@ -3825,7 +3801,7 @@
         <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74">
@@ -3865,7 +3841,7 @@
         <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79">
@@ -4081,7 +4057,7 @@
         <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106">
@@ -4097,7 +4073,7 @@
         <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108">
@@ -4113,7 +4089,7 @@
         <v>206</v>
       </c>
       <c r="B109" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110">
@@ -4129,7 +4105,7 @@
         <v>209</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112">
@@ -4169,7 +4145,7 @@
         <v>216</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117">
@@ -4337,7 +4313,7 @@
         <v>252</v>
       </c>
       <c r="B137" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="138">
@@ -4377,23 +4353,23 @@
         <v>261</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
         <v>263</v>
-      </c>
-      <c r="B143" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
+        <v>264</v>
+      </c>
+      <c r="B144" t="s">
         <v>265</v>
-      </c>
-      <c r="B144" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="145">
@@ -4425,23 +4401,23 @@
         <v>272</v>
       </c>
       <c r="B148" t="s">
-        <v>273</v>
+        <v>153</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
+        <v>273</v>
+      </c>
+      <c r="B149" t="s">
         <v>274</v>
-      </c>
-      <c r="B149" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
+        <v>275</v>
+      </c>
+      <c r="B150" t="s">
         <v>276</v>
-      </c>
-      <c r="B150" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="151">
@@ -4457,31 +4433,31 @@
         <v>279</v>
       </c>
       <c r="B152" t="s">
-        <v>280</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B153" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B154" t="s">
-        <v>111</v>
+        <v>282</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
+        <v>283</v>
+      </c>
+      <c r="B155" t="s">
         <v>284</v>
-      </c>
-      <c r="B155" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="156">
@@ -4489,39 +4465,39 @@
         <v>285</v>
       </c>
       <c r="B156" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
+        <v>286</v>
+      </c>
+      <c r="B157" t="s">
         <v>287</v>
-      </c>
-      <c r="B157" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B158" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>289</v>
+      </c>
+      <c r="B159" t="s">
         <v>290</v>
-      </c>
-      <c r="B159" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
+        <v>291</v>
+      </c>
+      <c r="B160" t="s">
         <v>292</v>
-      </c>
-      <c r="B160" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="161">
@@ -4537,47 +4513,47 @@
         <v>295</v>
       </c>
       <c r="B162" t="s">
-        <v>296</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B163" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B164" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B165" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B166" t="s">
-        <v>11</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
+        <v>303</v>
+      </c>
+      <c r="B167" t="s">
         <v>304</v>
-      </c>
-      <c r="B167" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="168">
@@ -4609,39 +4585,39 @@
         <v>311</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>44</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" t="s">
         <v>313</v>
-      </c>
-      <c r="B172" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
+        <v>314</v>
+      </c>
+      <c r="B173" t="s">
         <v>315</v>
-      </c>
-      <c r="B173" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>316</v>
+      </c>
+      <c r="B174" t="s">
         <v>317</v>
-      </c>
-      <c r="B174" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
+        <v>318</v>
+      </c>
+      <c r="B175" t="s">
         <v>319</v>
-      </c>
-      <c r="B175" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="176">
@@ -4649,39 +4625,39 @@
         <v>320</v>
       </c>
       <c r="B176" t="s">
-        <v>321</v>
+        <v>77</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
+        <v>321</v>
+      </c>
+      <c r="B177" t="s">
         <v>322</v>
-      </c>
-      <c r="B177" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" t="s">
         <v>324</v>
-      </c>
-      <c r="B178" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
+        <v>325</v>
+      </c>
+      <c r="B179" t="s">
         <v>326</v>
-      </c>
-      <c r="B179" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" t="s">
         <v>328</v>
-      </c>
-      <c r="B180" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="181">
@@ -4689,39 +4665,39 @@
         <v>329</v>
       </c>
       <c r="B181" t="s">
-        <v>330</v>
+        <v>113</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
+        <v>330</v>
+      </c>
+      <c r="B182" t="s">
         <v>331</v>
-      </c>
-      <c r="B182" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
+        <v>332</v>
+      </c>
+      <c r="B183" t="s">
         <v>333</v>
-      </c>
-      <c r="B183" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
+        <v>334</v>
+      </c>
+      <c r="B184" t="s">
         <v>335</v>
-      </c>
-      <c r="B184" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>336</v>
+      </c>
+      <c r="B185" t="s">
         <v>337</v>
-      </c>
-      <c r="B185" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="186">
@@ -4745,55 +4721,55 @@
         <v>342</v>
       </c>
       <c r="B188" t="s">
-        <v>343</v>
+        <v>103</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
+        <v>343</v>
+      </c>
+      <c r="B189" t="s">
         <v>344</v>
-      </c>
-      <c r="B189" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B190" t="s">
-        <v>347</v>
+        <v>222</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B191" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B192" t="s">
-        <v>101</v>
+        <v>349</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
+        <v>350</v>
+      </c>
+      <c r="B193" t="s">
         <v>351</v>
-      </c>
-      <c r="B193" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
+        <v>352</v>
+      </c>
+      <c r="B194" t="s">
         <v>353</v>
-      </c>
-      <c r="B194" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="195">
@@ -4865,39 +4841,39 @@
         <v>369</v>
       </c>
       <c r="B203" t="s">
-        <v>370</v>
+        <v>151</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B204" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B205" t="s">
-        <v>258</v>
+        <v>372</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
+        <v>373</v>
+      </c>
+      <c r="B206" t="s">
         <v>374</v>
-      </c>
-      <c r="B206" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
+        <v>375</v>
+      </c>
+      <c r="B207" t="s">
         <v>376</v>
-      </c>
-      <c r="B207" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="208">
@@ -4905,23 +4881,23 @@
         <v>377</v>
       </c>
       <c r="B208" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B209" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B210" t="s">
-        <v>381</v>
+        <v>107</v>
       </c>
     </row>
     <row r="211">
@@ -4953,47 +4929,47 @@
         <v>388</v>
       </c>
       <c r="B214" t="s">
-        <v>105</v>
+        <v>389</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B215" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B216" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B217" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B218" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B219" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220">
@@ -5025,23 +5001,23 @@
         <v>405</v>
       </c>
       <c r="B223" t="s">
-        <v>197</v>
+        <v>406</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B224" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B225" t="s">
-        <v>409</v>
+        <v>103</v>
       </c>
     </row>
     <row r="226">
@@ -5049,31 +5025,31 @@
         <v>410</v>
       </c>
       <c r="B226" t="s">
-        <v>411</v>
+        <v>113</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
-        <v>413</v>
+        <v>90</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B228" t="s">
-        <v>101</v>
+        <v>413</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
+        <v>414</v>
+      </c>
+      <c r="B229" t="s">
         <v>415</v>
-      </c>
-      <c r="B229" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="230">
@@ -5081,7 +5057,7 @@
         <v>416</v>
       </c>
       <c r="B230" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
     </row>
     <row r="231">
@@ -5105,7 +5081,7 @@
         <v>421</v>
       </c>
       <c r="B233" t="s">
-        <v>173</v>
+        <v>239</v>
       </c>
     </row>
     <row r="234">
@@ -5129,15 +5105,15 @@
         <v>426</v>
       </c>
       <c r="B236" t="s">
-        <v>239</v>
+        <v>427</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B237" t="s">
-        <v>428</v>
+        <v>151</v>
       </c>
     </row>
     <row r="238">
@@ -5145,15 +5121,15 @@
         <v>429</v>
       </c>
       <c r="B238" t="s">
-        <v>430</v>
+        <v>267</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
+        <v>430</v>
+      </c>
+      <c r="B239" t="s">
         <v>431</v>
-      </c>
-      <c r="B239" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="240">
@@ -5161,63 +5137,63 @@
         <v>432</v>
       </c>
       <c r="B240" t="s">
-        <v>271</v>
+        <v>433</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B241" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B242" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B243" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B244" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B245" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B246" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B247" t="s">
-        <v>446</v>
+        <v>129</v>
       </c>
     </row>
     <row r="248">
@@ -5233,7 +5209,7 @@
         <v>449</v>
       </c>
       <c r="B249" t="s">
-        <v>127</v>
+        <v>441</v>
       </c>
     </row>
     <row r="250">
@@ -5249,31 +5225,31 @@
         <v>452</v>
       </c>
       <c r="B251" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B252" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B253" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B254" t="s">
-        <v>458</v>
+        <v>267</v>
       </c>
     </row>
     <row r="255">
@@ -5281,31 +5257,31 @@
         <v>459</v>
       </c>
       <c r="B255" t="s">
-        <v>460</v>
+        <v>103</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B256" t="s">
-        <v>271</v>
+        <v>208</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B257" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
+        <v>462</v>
+      </c>
+      <c r="B258" t="s">
         <v>463</v>
-      </c>
-      <c r="B258" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="259">
@@ -5313,7 +5289,7 @@
         <v>464</v>
       </c>
       <c r="B259" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="260">
@@ -5321,47 +5297,47 @@
         <v>465</v>
       </c>
       <c r="B260" t="s">
-        <v>466</v>
+        <v>278</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B261" t="s">
-        <v>140</v>
+        <v>376</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B262" t="s">
-        <v>282</v>
+        <v>113</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B263" t="s">
-        <v>470</v>
+        <v>151</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B264" t="s">
-        <v>383</v>
+        <v>470</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
+        <v>471</v>
+      </c>
+      <c r="B265" t="s">
         <v>472</v>
-      </c>
-      <c r="B265" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="266">
@@ -5369,15 +5345,15 @@
         <v>473</v>
       </c>
       <c r="B266" t="s">
-        <v>151</v>
+        <v>474</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B267" t="s">
-        <v>475</v>
+        <v>113</v>
       </c>
     </row>
     <row r="268">
@@ -5401,7 +5377,7 @@
         <v>480</v>
       </c>
       <c r="B270" t="s">
-        <v>111</v>
+        <v>389</v>
       </c>
     </row>
     <row r="271">
@@ -5425,7 +5401,7 @@
         <v>485</v>
       </c>
       <c r="B273" t="s">
-        <v>396</v>
+        <v>113</v>
       </c>
     </row>
     <row r="274">
@@ -5441,39 +5417,39 @@
         <v>488</v>
       </c>
       <c r="B275" t="s">
-        <v>489</v>
+        <v>129</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B276" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B277" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B278" t="s">
-        <v>127</v>
+        <v>492</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
+        <v>493</v>
+      </c>
+      <c r="B279" t="s">
         <v>494</v>
-      </c>
-      <c r="B279" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="280">
@@ -5481,7 +5457,7 @@
         <v>495</v>
       </c>
       <c r="B280" t="s">
-        <v>477</v>
+        <v>239</v>
       </c>
     </row>
     <row r="281">
@@ -5489,31 +5465,31 @@
         <v>496</v>
       </c>
       <c r="B281" t="s">
-        <v>497</v>
+        <v>153</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
+        <v>497</v>
+      </c>
+      <c r="B282" t="s">
         <v>498</v>
-      </c>
-      <c r="B282" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B283" t="s">
-        <v>239</v>
+        <v>470</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
+        <v>500</v>
+      </c>
+      <c r="B284" t="s">
         <v>501</v>
-      </c>
-      <c r="B284" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="285">
@@ -5521,15 +5497,15 @@
         <v>502</v>
       </c>
       <c r="B285" t="s">
-        <v>503</v>
+        <v>208</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
+        <v>503</v>
+      </c>
+      <c r="B286" t="s">
         <v>504</v>
-      </c>
-      <c r="B286" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="287">
@@ -5545,7 +5521,7 @@
         <v>507</v>
       </c>
       <c r="B288" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
     </row>
     <row r="289">
@@ -5569,15 +5545,15 @@
         <v>512</v>
       </c>
       <c r="B291" t="s">
-        <v>167</v>
+        <v>513</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B292" t="s">
-        <v>514</v>
+        <v>142</v>
       </c>
     </row>
     <row r="293">
@@ -5585,23 +5561,23 @@
         <v>515</v>
       </c>
       <c r="B293" t="s">
-        <v>516</v>
+        <v>331</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
+        <v>516</v>
+      </c>
+      <c r="B294" t="s">
         <v>517</v>
-      </c>
-      <c r="B294" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
+        <v>518</v>
+      </c>
+      <c r="B295" t="s">
         <v>519</v>
-      </c>
-      <c r="B295" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="296">
@@ -5633,23 +5609,23 @@
         <v>526</v>
       </c>
       <c r="B299" t="s">
-        <v>527</v>
+        <v>153</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
+        <v>527</v>
+      </c>
+      <c r="B300" t="s">
         <v>528</v>
-      </c>
-      <c r="B300" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
+        <v>529</v>
+      </c>
+      <c r="B301" t="s">
         <v>530</v>
-      </c>
-      <c r="B301" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="302">
@@ -5673,119 +5649,119 @@
         <v>535</v>
       </c>
       <c r="B304" t="s">
-        <v>536</v>
+        <v>222</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B305" t="s">
-        <v>538</v>
+        <v>222</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B306" t="s">
-        <v>222</v>
+        <v>538</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B307" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="s">
+        <v>540</v>
+      </c>
+      <c r="B308" t="s">
         <v>541</v>
-      </c>
-      <c r="B308" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B309" t="s">
-        <v>247</v>
+        <v>153</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="s">
+        <v>543</v>
+      </c>
+      <c r="B310" t="s">
         <v>544</v>
-      </c>
-      <c r="B310" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B311" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B312" t="s">
-        <v>548</v>
+        <v>298</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B313" t="s">
-        <v>105</v>
+        <v>548</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B314" t="s">
-        <v>306</v>
+        <v>224</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="s">
+        <v>550</v>
+      </c>
+      <c r="B315" t="s">
         <v>551</v>
-      </c>
-      <c r="B315" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B316" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="s">
+        <v>553</v>
+      </c>
+      <c r="B317" t="s">
         <v>554</v>
-      </c>
-      <c r="B317" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="s">
+        <v>555</v>
+      </c>
+      <c r="B318" t="s">
         <v>556</v>
-      </c>
-      <c r="B318" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="319">
@@ -5793,39 +5769,39 @@
         <v>557</v>
       </c>
       <c r="B319" t="s">
-        <v>558</v>
+        <v>247</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B320" t="s">
-        <v>560</v>
+        <v>70</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B321" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B322" t="s">
-        <v>68</v>
+        <v>561</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="s">
+        <v>562</v>
+      </c>
+      <c r="B323" t="s">
         <v>563</v>
-      </c>
-      <c r="B323" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="324">
@@ -5833,23 +5809,23 @@
         <v>564</v>
       </c>
       <c r="B324" t="s">
-        <v>565</v>
+        <v>199</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="s">
+        <v>565</v>
+      </c>
+      <c r="B325" t="s">
         <v>566</v>
-      </c>
-      <c r="B325" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="s">
+        <v>567</v>
+      </c>
+      <c r="B326" t="s">
         <v>568</v>
-      </c>
-      <c r="B326" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="327">
@@ -5857,23 +5833,23 @@
         <v>569</v>
       </c>
       <c r="B327" t="s">
-        <v>570</v>
+        <v>441</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
+        <v>570</v>
+      </c>
+      <c r="B328" t="s">
         <v>571</v>
-      </c>
-      <c r="B328" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="s">
+        <v>572</v>
+      </c>
+      <c r="B329" t="s">
         <v>573</v>
-      </c>
-      <c r="B329" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="330">
@@ -5929,39 +5905,39 @@
         <v>586</v>
       </c>
       <c r="B336" t="s">
-        <v>587</v>
+        <v>302</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="s">
+        <v>587</v>
+      </c>
+      <c r="B337" t="s">
         <v>588</v>
-      </c>
-      <c r="B337" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B338" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="s">
+        <v>590</v>
+      </c>
+      <c r="B339" t="s">
         <v>591</v>
-      </c>
-      <c r="B339" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="s">
+        <v>592</v>
+      </c>
+      <c r="B340" t="s">
         <v>593</v>
-      </c>
-      <c r="B340" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="341">
@@ -5977,23 +5953,23 @@
         <v>596</v>
       </c>
       <c r="B342" t="s">
-        <v>597</v>
+        <v>328</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="s">
+        <v>597</v>
+      </c>
+      <c r="B343" t="s">
         <v>598</v>
-      </c>
-      <c r="B343" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="s">
+        <v>599</v>
+      </c>
+      <c r="B344" t="s">
         <v>600</v>
-      </c>
-      <c r="B344" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="345">
@@ -6001,119 +5977,119 @@
         <v>601</v>
       </c>
       <c r="B345" t="s">
-        <v>602</v>
+        <v>153</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B346" t="s">
-        <v>604</v>
+        <v>129</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B347" t="s">
-        <v>153</v>
+        <v>294</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B348" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B349" t="s">
-        <v>300</v>
+        <v>606</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B350" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B351" t="s">
-        <v>610</v>
+        <v>169</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B352" t="s">
-        <v>222</v>
+        <v>324</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B353" t="s">
-        <v>213</v>
+        <v>611</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B354" t="s">
-        <v>169</v>
+        <v>477</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B355" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B356" t="s">
-        <v>616</v>
+        <v>278</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B357" t="s">
-        <v>482</v>
+        <v>616</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B358" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="s">
+        <v>618</v>
+      </c>
+      <c r="B359" t="s">
         <v>619</v>
-      </c>
-      <c r="B359" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="360">
@@ -6129,15 +6105,15 @@
         <v>622</v>
       </c>
       <c r="B361" t="s">
-        <v>336</v>
+        <v>623</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B362" t="s">
-        <v>624</v>
+        <v>101</v>
       </c>
     </row>
     <row r="363">
@@ -6145,23 +6121,23 @@
         <v>625</v>
       </c>
       <c r="B363" t="s">
-        <v>626</v>
+        <v>251</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="s">
+        <v>626</v>
+      </c>
+      <c r="B364" t="s">
         <v>627</v>
-      </c>
-      <c r="B364" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="s">
+        <v>628</v>
+      </c>
+      <c r="B365" t="s">
         <v>629</v>
-      </c>
-      <c r="B365" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="366">
@@ -6169,47 +6145,47 @@
         <v>630</v>
       </c>
       <c r="B366" t="s">
-        <v>251</v>
+        <v>631</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B367" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B368" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B369" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B370" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B371" t="s">
-        <v>640</v>
+        <v>224</v>
       </c>
     </row>
     <row r="372">
@@ -6217,23 +6193,23 @@
         <v>641</v>
       </c>
       <c r="B372" t="s">
-        <v>642</v>
+        <v>77</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
+        <v>642</v>
+      </c>
+      <c r="B373" t="s">
         <v>643</v>
-      </c>
-      <c r="B373" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
+        <v>644</v>
+      </c>
+      <c r="B374" t="s">
         <v>645</v>
-      </c>
-      <c r="B374" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="375">
@@ -6241,7 +6217,7 @@
         <v>646</v>
       </c>
       <c r="B375" t="s">
-        <v>75</v>
+        <v>439</v>
       </c>
     </row>
     <row r="376">
@@ -6249,15 +6225,15 @@
         <v>647</v>
       </c>
       <c r="B376" t="s">
-        <v>648</v>
+        <v>205</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="s">
+        <v>648</v>
+      </c>
+      <c r="B377" t="s">
         <v>649</v>
-      </c>
-      <c r="B377" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="378">
@@ -6265,15 +6241,15 @@
         <v>650</v>
       </c>
       <c r="B378" t="s">
-        <v>651</v>
+        <v>239</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="s">
+        <v>651</v>
+      </c>
+      <c r="B379" t="s">
         <v>652</v>
-      </c>
-      <c r="B379" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="380">
@@ -6281,15 +6257,15 @@
         <v>653</v>
       </c>
       <c r="B380" t="s">
-        <v>205</v>
+        <v>654</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B381" t="s">
-        <v>655</v>
+        <v>113</v>
       </c>
     </row>
     <row r="382">
@@ -6297,15 +6273,15 @@
         <v>656</v>
       </c>
       <c r="B382" t="s">
-        <v>239</v>
+        <v>657</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B383" t="s">
-        <v>658</v>
+        <v>302</v>
       </c>
     </row>
     <row r="384">
@@ -6321,7 +6297,7 @@
         <v>661</v>
       </c>
       <c r="B385" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
     </row>
     <row r="386">
@@ -6329,39 +6305,39 @@
         <v>662</v>
       </c>
       <c r="B386" t="s">
-        <v>663</v>
+        <v>220</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B387" t="s">
-        <v>310</v>
+        <v>521</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="s">
+        <v>664</v>
+      </c>
+      <c r="B388" t="s">
         <v>665</v>
-      </c>
-      <c r="B388" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B389" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
+        <v>667</v>
+      </c>
+      <c r="B390" t="s">
         <v>668</v>
-      </c>
-      <c r="B390" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="391">
@@ -6369,7 +6345,7 @@
         <v>669</v>
       </c>
       <c r="B391" t="s">
-        <v>525</v>
+        <v>153</v>
       </c>
     </row>
     <row r="392">
@@ -6377,15 +6353,15 @@
         <v>670</v>
       </c>
       <c r="B392" t="s">
-        <v>671</v>
+        <v>455</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="s">
+        <v>671</v>
+      </c>
+      <c r="B393" t="s">
         <v>672</v>
-      </c>
-      <c r="B393" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="394">
@@ -6401,63 +6377,63 @@
         <v>675</v>
       </c>
       <c r="B395" t="s">
-        <v>676</v>
+        <v>77</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B396" t="s">
-        <v>153</v>
+        <v>319</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B397" t="s">
-        <v>458</v>
+        <v>34</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="s">
+        <v>678</v>
+      </c>
+      <c r="B398" t="s">
         <v>679</v>
-      </c>
-      <c r="B398" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="s">
+        <v>680</v>
+      </c>
+      <c r="B399" t="s">
         <v>681</v>
-      </c>
-      <c r="B399" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B400" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B401" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="s">
+        <v>684</v>
+      </c>
+      <c r="B402" t="s">
         <v>685</v>
-      </c>
-      <c r="B402" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="403">
@@ -6473,15 +6449,15 @@
         <v>688</v>
       </c>
       <c r="B404" t="s">
-        <v>689</v>
+        <v>298</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="s">
+        <v>689</v>
+      </c>
+      <c r="B405" t="s">
         <v>690</v>
-      </c>
-      <c r="B405" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="406">
@@ -6489,7 +6465,7 @@
         <v>691</v>
       </c>
       <c r="B406" t="s">
-        <v>339</v>
+        <v>687</v>
       </c>
     </row>
     <row r="407">
@@ -6505,15 +6481,15 @@
         <v>694</v>
       </c>
       <c r="B408" t="s">
-        <v>695</v>
+        <v>470</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="s">
+        <v>695</v>
+      </c>
+      <c r="B409" t="s">
         <v>696</v>
-      </c>
-      <c r="B409" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="410">
@@ -6521,55 +6497,55 @@
         <v>697</v>
       </c>
       <c r="B410" t="s">
-        <v>698</v>
+        <v>90</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B411" t="s">
-        <v>695</v>
+        <v>308</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="s">
+        <v>699</v>
+      </c>
+      <c r="B412" t="s">
         <v>700</v>
-      </c>
-      <c r="B412" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B413" t="s">
-        <v>475</v>
+        <v>103</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B414" t="s">
-        <v>704</v>
+        <v>129</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B415" t="s">
-        <v>88</v>
+        <v>704</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="s">
+        <v>705</v>
+      </c>
+      <c r="B416" t="s">
         <v>706</v>
-      </c>
-      <c r="B416" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="417">
@@ -6577,23 +6553,23 @@
         <v>707</v>
       </c>
       <c r="B417" t="s">
-        <v>708</v>
+        <v>119</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B418" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
+        <v>709</v>
+      </c>
+      <c r="B419" t="s">
         <v>710</v>
-      </c>
-      <c r="B419" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="420">
@@ -6601,23 +6577,23 @@
         <v>711</v>
       </c>
       <c r="B420" t="s">
-        <v>712</v>
+        <v>681</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
+        <v>712</v>
+      </c>
+      <c r="B421" t="s">
         <v>713</v>
-      </c>
-      <c r="B421" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
+        <v>714</v>
+      </c>
+      <c r="B422" t="s">
         <v>715</v>
-      </c>
-      <c r="B422" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="423">
@@ -6625,263 +6601,223 @@
         <v>716</v>
       </c>
       <c r="B423" t="s">
-        <v>111</v>
+        <v>717</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>717</v>
+        <v>95</v>
       </c>
       <c r="B424" t="s">
-        <v>718</v>
+        <v>96</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
-        <v>719</v>
+        <v>106</v>
       </c>
       <c r="B425" t="s">
-        <v>689</v>
+        <v>718</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
+        <v>719</v>
+      </c>
+      <c r="B426" t="s">
         <v>720</v>
-      </c>
-      <c r="B426" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B427" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B428" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="B429" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
-        <v>104</v>
+        <v>723</v>
       </c>
       <c r="B430" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B431" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B432" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B433" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
-        <v>214</v>
+        <v>360</v>
       </c>
       <c r="B434" t="s">
-        <v>215</v>
+        <v>361</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
-        <v>731</v>
+        <v>399</v>
       </c>
       <c r="B435" t="s">
-        <v>723</v>
+        <v>400</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
-        <v>732</v>
+        <v>401</v>
       </c>
       <c r="B436" t="s">
-        <v>723</v>
+        <v>402</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="B437" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
-        <v>734</v>
+        <v>412</v>
       </c>
       <c r="B438" t="s">
-        <v>735</v>
+        <v>413</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
-        <v>367</v>
+        <v>432</v>
       </c>
       <c r="B439" t="s">
-        <v>368</v>
+        <v>729</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
-        <v>406</v>
+        <v>436</v>
       </c>
       <c r="B440" t="s">
-        <v>407</v>
+        <v>437</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
-        <v>408</v>
+        <v>730</v>
       </c>
       <c r="B441" t="s">
-        <v>409</v>
+        <v>715</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
-        <v>736</v>
+        <v>574</v>
       </c>
       <c r="B442" t="s">
-        <v>723</v>
+        <v>575</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
-        <v>417</v>
+        <v>628</v>
       </c>
       <c r="B443" t="s">
-        <v>418</v>
+        <v>629</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
-        <v>435</v>
+        <v>731</v>
       </c>
       <c r="B444" t="s">
-        <v>737</v>
+        <v>715</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
-        <v>439</v>
+        <v>732</v>
       </c>
       <c r="B445" t="s">
-        <v>440</v>
+        <v>715</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="B446" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
-        <v>578</v>
+        <v>644</v>
       </c>
       <c r="B447" t="s">
-        <v>579</v>
+        <v>645</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
-        <v>633</v>
+        <v>734</v>
       </c>
       <c r="B448" t="s">
-        <v>634</v>
+        <v>715</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="B449" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B450" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" t="s">
-        <v>741</v>
-      </c>
-      <c r="B451" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" t="s">
-        <v>650</v>
-      </c>
-      <c r="B452" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" t="s">
-        <v>742</v>
-      </c>
-      <c r="B453" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" t="s">
-        <v>743</v>
-      </c>
-      <c r="B454" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" t="s">
-        <v>744</v>
-      </c>
-      <c r="B455" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -6900,7 +6836,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6908,31 +6844,31 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="B2" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B3" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="B4" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
@@ -6940,319 +6876,319 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="B6" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="B7" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="B9" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="B10" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="B11" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="B12" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="B13" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="B14" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="B15" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B16" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="B17" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="B19" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B21" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="B22" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B23" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="B25" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="B26" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="B27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B28" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="B29" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="B31" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="B32" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="B35" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="B36" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="B37" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="B38" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="B39" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B40" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="B41" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B42" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B44" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="B45" t="s">
         <v>224</v>
@@ -7260,119 +7196,119 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="B46" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="B47" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="B48" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="B49" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B50" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="B51" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="B52" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="B53" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="B54" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="B55" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="B56" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="B57" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="B58" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="B59" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="B60" t="s">
         <v>32</v>
@@ -7380,143 +7316,143 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="B61" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="B62" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="B63" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="B64" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="B65" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="B66" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="B67" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="B68" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="B69" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="B70" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="B71" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="B73" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B74" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="B75" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="B76" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="B77" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="B78" t="s">
         <v>171</v>
@@ -7524,47 +7460,47 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="B79" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="B80" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="B81" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="B82" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="B83" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="B84" t="s">
         <v>220</v>
@@ -7572,23 +7508,23 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="B85" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="B86" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="B87" t="s">
         <v>17</v>
@@ -7596,10 +7532,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -7618,68 +7554,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="B2" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="C2" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="B3" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C3" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="B4" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="C4" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="B5" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="C5" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="B6" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="C6" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -7698,332 +7634,332 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="B3" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="C3" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="B4" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="C4" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="B5" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="C5" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="B6" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="C6" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B8" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C8" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="B9" t="s">
         <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="B10" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="C10" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="B11" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="C11" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="B13" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="C13" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="B14" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="C14" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="B15" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="C15" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="B16" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="C16" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="B17" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="C17" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="B20" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="C20" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="B21" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="C21" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="B22" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="C22" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="B24" t="s">
         <v>222</v>
       </c>
       <c r="C24" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="B25" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C25" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="B26" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="C26" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="B27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C27" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="B28" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="C28" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="B29" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="C29" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>964</v>
+        <v>956</v>
       </c>
       <c r="B30" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="C30" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revision: Update Table 1 to include Patient Ns (#1643)
* Update Table 1 to include patient-level Ns

* rerun with v22

* fix table 1 headers

* update table run to release v23

Co-authored-by: Jaclyn Taroni <19534205+jaclyn-taroni@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tables/results/TableS5-Key-Resources-table.xlsx
+++ b/tables/results/TableS5-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="958">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -134,6 +134,12 @@
     <t xml:space="preserve">1.0.7</t>
   </si>
   <si>
+    <t xml:space="preserve">berryFunctions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.18.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BH</t>
   </si>
   <si>
@@ -413,12 +419,6 @@
     <t xml:space="preserve">0.8.5</t>
   </si>
   <si>
-    <t xml:space="preserve">d3treeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">data.table</t>
   </si>
   <si>
@@ -782,342 +782,321 @@
     <t xml:space="preserve">1.34.0</t>
   </si>
   <si>
-    <t xml:space="preserve">ggfittext</t>
+    <t xml:space="preserve">ggforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggfortify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggplot2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggpubr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggrepel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggsci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggsignif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggthemes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggupset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1.0.9000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git2r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glmnetUtils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobalOptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmailr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5-13.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gplots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridExtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gridGraphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSEABase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hexbin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.27.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4.7.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hmisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmlTable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.13.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmltools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htmlwidgets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">httpuv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">httr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hunspell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hwriter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">igraph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">immunedeconv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">influenceR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interactiveDisplayBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.24.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ipred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRanges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.20.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iterators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">janitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jsonlite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kknn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km.ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMsurv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knitr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lahman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">later</t>
   </si>
   <si>
     <t xml:space="preserve">0.8.0</t>
   </si>
   <si>
-    <t xml:space="preserve">ggforce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggfortify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggpattern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggplot2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggpubr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggrepel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggsci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggsignif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggthemes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ggupset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1.0.9000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git2r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glmnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glmnetUtils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GlobalOptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmailr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5-13.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gplots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridBase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridExtra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridGeometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridGraphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridSVG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSEABase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gtable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gtools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">haven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hexbin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.27.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highlight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4.7.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hmisc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmlTable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.13.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmltools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">htmlwidgets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">httpuv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">httr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hunspell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hwriter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">igraph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">immunedeconv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">influenceR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interactiveDisplayBase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.24.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ipred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRanges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.20.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iterators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">janitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jsonlite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kknn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">km.ci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMsurv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">knitr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labeling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lahman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda.r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">later</t>
-  </si>
-  <si>
     <t xml:space="preserve">lattice</t>
   </si>
   <si>
@@ -1259,6 +1238,12 @@
     <t xml:space="preserve">0.7-25</t>
   </si>
   <si>
+    <t xml:space="preserve">mclust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.4.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">MCPcounter</t>
   </si>
   <si>
@@ -1310,6 +1295,12 @@
     <t xml:space="preserve">6.2.1</t>
   </si>
   <si>
+    <t xml:space="preserve">MultiAssayExperiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.10.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">multipanelfigure</t>
   </si>
   <si>
@@ -1424,12 +1415,6 @@
     <t xml:space="preserve">pingr</t>
   </si>
   <si>
-    <t xml:space="preserve">pipeR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6.1.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">pkgbuild</t>
   </si>
   <si>
@@ -1574,6 +1559,9 @@
     <t xml:space="preserve">2.4.0</t>
   </si>
   <si>
+    <t xml:space="preserve">RaggedExperiment</t>
+  </si>
+  <si>
     <t xml:space="preserve">rappdirs</t>
   </si>
   <si>
@@ -1850,9 +1838,6 @@
     <t xml:space="preserve">0.7-5</t>
   </si>
   <si>
-    <t xml:space="preserve">shades</t>
-  </si>
-  <si>
     <t xml:space="preserve">shape</t>
   </si>
   <si>
@@ -1964,9 +1949,6 @@
     <t xml:space="preserve">1.16.1</t>
   </si>
   <si>
-    <t xml:space="preserve">sunburstR</t>
-  </si>
-  <si>
     <t xml:space="preserve">survival</t>
   </si>
   <si>
@@ -2040,12 +2022,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.4-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treemapify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5.2</t>
   </si>
   <si>
     <t xml:space="preserve">tweenr</t>
@@ -3529,15 +3505,15 @@
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
@@ -3569,31 +3545,31 @@
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45">
@@ -3657,15 +3633,15 @@
         <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54">
@@ -3825,7 +3801,7 @@
         <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74">
@@ -3865,7 +3841,7 @@
         <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79">
@@ -4081,7 +4057,7 @@
         <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106">
@@ -4097,7 +4073,7 @@
         <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108">
@@ -4113,7 +4089,7 @@
         <v>206</v>
       </c>
       <c r="B109" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110">
@@ -4129,7 +4105,7 @@
         <v>209</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112">
@@ -4169,7 +4145,7 @@
         <v>216</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117">
@@ -4337,7 +4313,7 @@
         <v>252</v>
       </c>
       <c r="B137" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="138">
@@ -4377,23 +4353,23 @@
         <v>261</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
         <v>263</v>
-      </c>
-      <c r="B143" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
+        <v>264</v>
+      </c>
+      <c r="B144" t="s">
         <v>265</v>
-      </c>
-      <c r="B144" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="145">
@@ -4425,23 +4401,23 @@
         <v>272</v>
       </c>
       <c r="B148" t="s">
-        <v>273</v>
+        <v>153</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
+        <v>273</v>
+      </c>
+      <c r="B149" t="s">
         <v>274</v>
-      </c>
-      <c r="B149" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
+        <v>275</v>
+      </c>
+      <c r="B150" t="s">
         <v>276</v>
-      </c>
-      <c r="B150" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="151">
@@ -4457,31 +4433,31 @@
         <v>279</v>
       </c>
       <c r="B152" t="s">
-        <v>280</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B153" t="s">
-        <v>282</v>
+        <v>222</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B154" t="s">
-        <v>111</v>
+        <v>282</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
+        <v>283</v>
+      </c>
+      <c r="B155" t="s">
         <v>284</v>
-      </c>
-      <c r="B155" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="156">
@@ -4489,39 +4465,39 @@
         <v>285</v>
       </c>
       <c r="B156" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
+        <v>286</v>
+      </c>
+      <c r="B157" t="s">
         <v>287</v>
-      </c>
-      <c r="B157" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B158" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>289</v>
+      </c>
+      <c r="B159" t="s">
         <v>290</v>
-      </c>
-      <c r="B159" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
+        <v>291</v>
+      </c>
+      <c r="B160" t="s">
         <v>292</v>
-      </c>
-      <c r="B160" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="161">
@@ -4537,47 +4513,47 @@
         <v>295</v>
       </c>
       <c r="B162" t="s">
-        <v>296</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B163" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B164" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B165" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B166" t="s">
-        <v>11</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
+        <v>303</v>
+      </c>
+      <c r="B167" t="s">
         <v>304</v>
-      </c>
-      <c r="B167" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="168">
@@ -4609,39 +4585,39 @@
         <v>311</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>44</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" t="s">
         <v>313</v>
-      </c>
-      <c r="B172" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
+        <v>314</v>
+      </c>
+      <c r="B173" t="s">
         <v>315</v>
-      </c>
-      <c r="B173" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>316</v>
+      </c>
+      <c r="B174" t="s">
         <v>317</v>
-      </c>
-      <c r="B174" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
+        <v>318</v>
+      </c>
+      <c r="B175" t="s">
         <v>319</v>
-      </c>
-      <c r="B175" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="176">
@@ -4649,39 +4625,39 @@
         <v>320</v>
       </c>
       <c r="B176" t="s">
-        <v>321</v>
+        <v>77</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
+        <v>321</v>
+      </c>
+      <c r="B177" t="s">
         <v>322</v>
-      </c>
-      <c r="B177" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" t="s">
         <v>324</v>
-      </c>
-      <c r="B178" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
+        <v>325</v>
+      </c>
+      <c r="B179" t="s">
         <v>326</v>
-      </c>
-      <c r="B179" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" t="s">
         <v>328</v>
-      </c>
-      <c r="B180" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="181">
@@ -4689,39 +4665,39 @@
         <v>329</v>
       </c>
       <c r="B181" t="s">
-        <v>330</v>
+        <v>113</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
+        <v>330</v>
+      </c>
+      <c r="B182" t="s">
         <v>331</v>
-      </c>
-      <c r="B182" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
+        <v>332</v>
+      </c>
+      <c r="B183" t="s">
         <v>333</v>
-      </c>
-      <c r="B183" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
+        <v>334</v>
+      </c>
+      <c r="B184" t="s">
         <v>335</v>
-      </c>
-      <c r="B184" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>336</v>
+      </c>
+      <c r="B185" t="s">
         <v>337</v>
-      </c>
-      <c r="B185" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="186">
@@ -4745,55 +4721,55 @@
         <v>342</v>
       </c>
       <c r="B188" t="s">
-        <v>343</v>
+        <v>103</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
+        <v>343</v>
+      </c>
+      <c r="B189" t="s">
         <v>344</v>
-      </c>
-      <c r="B189" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B190" t="s">
-        <v>347</v>
+        <v>222</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B191" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B192" t="s">
-        <v>101</v>
+        <v>349</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
+        <v>350</v>
+      </c>
+      <c r="B193" t="s">
         <v>351</v>
-      </c>
-      <c r="B193" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
+        <v>352</v>
+      </c>
+      <c r="B194" t="s">
         <v>353</v>
-      </c>
-      <c r="B194" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="195">
@@ -4865,39 +4841,39 @@
         <v>369</v>
       </c>
       <c r="B203" t="s">
-        <v>370</v>
+        <v>151</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B204" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B205" t="s">
-        <v>258</v>
+        <v>372</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
+        <v>373</v>
+      </c>
+      <c r="B206" t="s">
         <v>374</v>
-      </c>
-      <c r="B206" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
+        <v>375</v>
+      </c>
+      <c r="B207" t="s">
         <v>376</v>
-      </c>
-      <c r="B207" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="208">
@@ -4905,23 +4881,23 @@
         <v>377</v>
       </c>
       <c r="B208" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B209" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B210" t="s">
-        <v>381</v>
+        <v>107</v>
       </c>
     </row>
     <row r="211">
@@ -4953,47 +4929,47 @@
         <v>388</v>
       </c>
       <c r="B214" t="s">
-        <v>105</v>
+        <v>389</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B215" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B216" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B217" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B218" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B219" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220">
@@ -5025,23 +5001,23 @@
         <v>405</v>
       </c>
       <c r="B223" t="s">
-        <v>197</v>
+        <v>406</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B224" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B225" t="s">
-        <v>409</v>
+        <v>103</v>
       </c>
     </row>
     <row r="226">
@@ -5049,31 +5025,31 @@
         <v>410</v>
       </c>
       <c r="B226" t="s">
-        <v>411</v>
+        <v>113</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
-        <v>413</v>
+        <v>90</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B228" t="s">
-        <v>101</v>
+        <v>413</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
+        <v>414</v>
+      </c>
+      <c r="B229" t="s">
         <v>415</v>
-      </c>
-      <c r="B229" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="230">
@@ -5081,7 +5057,7 @@
         <v>416</v>
       </c>
       <c r="B230" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
     </row>
     <row r="231">
@@ -5105,7 +5081,7 @@
         <v>421</v>
       </c>
       <c r="B233" t="s">
-        <v>173</v>
+        <v>239</v>
       </c>
     </row>
     <row r="234">
@@ -5129,15 +5105,15 @@
         <v>426</v>
       </c>
       <c r="B236" t="s">
-        <v>239</v>
+        <v>427</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B237" t="s">
-        <v>428</v>
+        <v>151</v>
       </c>
     </row>
     <row r="238">
@@ -5145,15 +5121,15 @@
         <v>429</v>
       </c>
       <c r="B238" t="s">
-        <v>430</v>
+        <v>267</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
+        <v>430</v>
+      </c>
+      <c r="B239" t="s">
         <v>431</v>
-      </c>
-      <c r="B239" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="240">
@@ -5161,63 +5137,63 @@
         <v>432</v>
       </c>
       <c r="B240" t="s">
-        <v>271</v>
+        <v>433</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B241" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B242" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B243" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B244" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B245" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B246" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B247" t="s">
-        <v>446</v>
+        <v>129</v>
       </c>
     </row>
     <row r="248">
@@ -5233,7 +5209,7 @@
         <v>449</v>
       </c>
       <c r="B249" t="s">
-        <v>127</v>
+        <v>441</v>
       </c>
     </row>
     <row r="250">
@@ -5249,31 +5225,31 @@
         <v>452</v>
       </c>
       <c r="B251" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B252" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B253" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B254" t="s">
-        <v>458</v>
+        <v>267</v>
       </c>
     </row>
     <row r="255">
@@ -5281,31 +5257,31 @@
         <v>459</v>
       </c>
       <c r="B255" t="s">
-        <v>460</v>
+        <v>103</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B256" t="s">
-        <v>271</v>
+        <v>208</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B257" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
+        <v>462</v>
+      </c>
+      <c r="B258" t="s">
         <v>463</v>
-      </c>
-      <c r="B258" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="259">
@@ -5313,7 +5289,7 @@
         <v>464</v>
       </c>
       <c r="B259" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="260">
@@ -5321,47 +5297,47 @@
         <v>465</v>
       </c>
       <c r="B260" t="s">
-        <v>466</v>
+        <v>278</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B261" t="s">
-        <v>140</v>
+        <v>376</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B262" t="s">
-        <v>282</v>
+        <v>113</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B263" t="s">
-        <v>470</v>
+        <v>151</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B264" t="s">
-        <v>383</v>
+        <v>470</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
+        <v>471</v>
+      </c>
+      <c r="B265" t="s">
         <v>472</v>
-      </c>
-      <c r="B265" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="266">
@@ -5369,15 +5345,15 @@
         <v>473</v>
       </c>
       <c r="B266" t="s">
-        <v>151</v>
+        <v>474</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B267" t="s">
-        <v>475</v>
+        <v>113</v>
       </c>
     </row>
     <row r="268">
@@ -5401,7 +5377,7 @@
         <v>480</v>
       </c>
       <c r="B270" t="s">
-        <v>111</v>
+        <v>389</v>
       </c>
     </row>
     <row r="271">
@@ -5425,7 +5401,7 @@
         <v>485</v>
       </c>
       <c r="B273" t="s">
-        <v>396</v>
+        <v>113</v>
       </c>
     </row>
     <row r="274">
@@ -5441,39 +5417,39 @@
         <v>488</v>
       </c>
       <c r="B275" t="s">
-        <v>489</v>
+        <v>129</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B276" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B277" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B278" t="s">
-        <v>127</v>
+        <v>492</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
+        <v>493</v>
+      </c>
+      <c r="B279" t="s">
         <v>494</v>
-      </c>
-      <c r="B279" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="280">
@@ -5481,7 +5457,7 @@
         <v>495</v>
       </c>
       <c r="B280" t="s">
-        <v>477</v>
+        <v>239</v>
       </c>
     </row>
     <row r="281">
@@ -5489,31 +5465,31 @@
         <v>496</v>
       </c>
       <c r="B281" t="s">
-        <v>497</v>
+        <v>153</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
+        <v>497</v>
+      </c>
+      <c r="B282" t="s">
         <v>498</v>
-      </c>
-      <c r="B282" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B283" t="s">
-        <v>239</v>
+        <v>470</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
+        <v>500</v>
+      </c>
+      <c r="B284" t="s">
         <v>501</v>
-      </c>
-      <c r="B284" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="285">
@@ -5521,15 +5497,15 @@
         <v>502</v>
       </c>
       <c r="B285" t="s">
-        <v>503</v>
+        <v>208</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
+        <v>503</v>
+      </c>
+      <c r="B286" t="s">
         <v>504</v>
-      </c>
-      <c r="B286" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="287">
@@ -5545,7 +5521,7 @@
         <v>507</v>
       </c>
       <c r="B288" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
     </row>
     <row r="289">
@@ -5569,15 +5545,15 @@
         <v>512</v>
       </c>
       <c r="B291" t="s">
-        <v>167</v>
+        <v>513</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B292" t="s">
-        <v>514</v>
+        <v>142</v>
       </c>
     </row>
     <row r="293">
@@ -5585,23 +5561,23 @@
         <v>515</v>
       </c>
       <c r="B293" t="s">
-        <v>516</v>
+        <v>331</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
+        <v>516</v>
+      </c>
+      <c r="B294" t="s">
         <v>517</v>
-      </c>
-      <c r="B294" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
+        <v>518</v>
+      </c>
+      <c r="B295" t="s">
         <v>519</v>
-      </c>
-      <c r="B295" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="296">
@@ -5633,23 +5609,23 @@
         <v>526</v>
       </c>
       <c r="B299" t="s">
-        <v>527</v>
+        <v>153</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
+        <v>527</v>
+      </c>
+      <c r="B300" t="s">
         <v>528</v>
-      </c>
-      <c r="B300" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
+        <v>529</v>
+      </c>
+      <c r="B301" t="s">
         <v>530</v>
-      </c>
-      <c r="B301" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="302">
@@ -5673,119 +5649,119 @@
         <v>535</v>
       </c>
       <c r="B304" t="s">
-        <v>536</v>
+        <v>222</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B305" t="s">
-        <v>538</v>
+        <v>222</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B306" t="s">
-        <v>222</v>
+        <v>538</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B307" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="s">
+        <v>540</v>
+      </c>
+      <c r="B308" t="s">
         <v>541</v>
-      </c>
-      <c r="B308" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B309" t="s">
-        <v>247</v>
+        <v>153</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="s">
+        <v>543</v>
+      </c>
+      <c r="B310" t="s">
         <v>544</v>
-      </c>
-      <c r="B310" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B311" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B312" t="s">
-        <v>548</v>
+        <v>298</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B313" t="s">
-        <v>105</v>
+        <v>548</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B314" t="s">
-        <v>306</v>
+        <v>224</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="s">
+        <v>550</v>
+      </c>
+      <c r="B315" t="s">
         <v>551</v>
-      </c>
-      <c r="B315" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B316" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="s">
+        <v>553</v>
+      </c>
+      <c r="B317" t="s">
         <v>554</v>
-      </c>
-      <c r="B317" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="s">
+        <v>555</v>
+      </c>
+      <c r="B318" t="s">
         <v>556</v>
-      </c>
-      <c r="B318" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="319">
@@ -5793,39 +5769,39 @@
         <v>557</v>
       </c>
       <c r="B319" t="s">
-        <v>558</v>
+        <v>247</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B320" t="s">
-        <v>560</v>
+        <v>70</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B321" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B322" t="s">
-        <v>68</v>
+        <v>561</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="s">
+        <v>562</v>
+      </c>
+      <c r="B323" t="s">
         <v>563</v>
-      </c>
-      <c r="B323" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="324">
@@ -5833,23 +5809,23 @@
         <v>564</v>
       </c>
       <c r="B324" t="s">
-        <v>565</v>
+        <v>199</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="s">
+        <v>565</v>
+      </c>
+      <c r="B325" t="s">
         <v>566</v>
-      </c>
-      <c r="B325" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="s">
+        <v>567</v>
+      </c>
+      <c r="B326" t="s">
         <v>568</v>
-      </c>
-      <c r="B326" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="327">
@@ -5857,23 +5833,23 @@
         <v>569</v>
       </c>
       <c r="B327" t="s">
-        <v>570</v>
+        <v>441</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
+        <v>570</v>
+      </c>
+      <c r="B328" t="s">
         <v>571</v>
-      </c>
-      <c r="B328" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="s">
+        <v>572</v>
+      </c>
+      <c r="B329" t="s">
         <v>573</v>
-      </c>
-      <c r="B329" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="330">
@@ -5929,39 +5905,39 @@
         <v>586</v>
       </c>
       <c r="B336" t="s">
-        <v>587</v>
+        <v>302</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="s">
+        <v>587</v>
+      </c>
+      <c r="B337" t="s">
         <v>588</v>
-      </c>
-      <c r="B337" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B338" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="s">
+        <v>590</v>
+      </c>
+      <c r="B339" t="s">
         <v>591</v>
-      </c>
-      <c r="B339" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="s">
+        <v>592</v>
+      </c>
+      <c r="B340" t="s">
         <v>593</v>
-      </c>
-      <c r="B340" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="341">
@@ -5977,23 +5953,23 @@
         <v>596</v>
       </c>
       <c r="B342" t="s">
-        <v>597</v>
+        <v>328</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="s">
+        <v>597</v>
+      </c>
+      <c r="B343" t="s">
         <v>598</v>
-      </c>
-      <c r="B343" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="s">
+        <v>599</v>
+      </c>
+      <c r="B344" t="s">
         <v>600</v>
-      </c>
-      <c r="B344" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="345">
@@ -6001,119 +5977,119 @@
         <v>601</v>
       </c>
       <c r="B345" t="s">
-        <v>602</v>
+        <v>153</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B346" t="s">
-        <v>604</v>
+        <v>129</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B347" t="s">
-        <v>153</v>
+        <v>294</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B348" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B349" t="s">
-        <v>300</v>
+        <v>606</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B350" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B351" t="s">
-        <v>610</v>
+        <v>169</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B352" t="s">
-        <v>222</v>
+        <v>324</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B353" t="s">
-        <v>213</v>
+        <v>611</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B354" t="s">
-        <v>169</v>
+        <v>477</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B355" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B356" t="s">
-        <v>616</v>
+        <v>278</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B357" t="s">
-        <v>482</v>
+        <v>616</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B358" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="s">
+        <v>618</v>
+      </c>
+      <c r="B359" t="s">
         <v>619</v>
-      </c>
-      <c r="B359" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="360">
@@ -6129,15 +6105,15 @@
         <v>622</v>
       </c>
       <c r="B361" t="s">
-        <v>336</v>
+        <v>623</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B362" t="s">
-        <v>624</v>
+        <v>101</v>
       </c>
     </row>
     <row r="363">
@@ -6145,23 +6121,23 @@
         <v>625</v>
       </c>
       <c r="B363" t="s">
-        <v>626</v>
+        <v>251</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="s">
+        <v>626</v>
+      </c>
+      <c r="B364" t="s">
         <v>627</v>
-      </c>
-      <c r="B364" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="s">
+        <v>628</v>
+      </c>
+      <c r="B365" t="s">
         <v>629</v>
-      </c>
-      <c r="B365" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="366">
@@ -6169,47 +6145,47 @@
         <v>630</v>
       </c>
       <c r="B366" t="s">
-        <v>251</v>
+        <v>631</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B367" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B368" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B369" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B370" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B371" t="s">
-        <v>640</v>
+        <v>224</v>
       </c>
     </row>
     <row r="372">
@@ -6217,23 +6193,23 @@
         <v>641</v>
       </c>
       <c r="B372" t="s">
-        <v>642</v>
+        <v>77</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
+        <v>642</v>
+      </c>
+      <c r="B373" t="s">
         <v>643</v>
-      </c>
-      <c r="B373" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
+        <v>644</v>
+      </c>
+      <c r="B374" t="s">
         <v>645</v>
-      </c>
-      <c r="B374" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="375">
@@ -6241,7 +6217,7 @@
         <v>646</v>
       </c>
       <c r="B375" t="s">
-        <v>75</v>
+        <v>439</v>
       </c>
     </row>
     <row r="376">
@@ -6249,15 +6225,15 @@
         <v>647</v>
       </c>
       <c r="B376" t="s">
-        <v>648</v>
+        <v>205</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="s">
+        <v>648</v>
+      </c>
+      <c r="B377" t="s">
         <v>649</v>
-      </c>
-      <c r="B377" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="378">
@@ -6265,15 +6241,15 @@
         <v>650</v>
       </c>
       <c r="B378" t="s">
-        <v>651</v>
+        <v>239</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="s">
+        <v>651</v>
+      </c>
+      <c r="B379" t="s">
         <v>652</v>
-      </c>
-      <c r="B379" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="380">
@@ -6281,15 +6257,15 @@
         <v>653</v>
       </c>
       <c r="B380" t="s">
-        <v>205</v>
+        <v>654</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B381" t="s">
-        <v>655</v>
+        <v>113</v>
       </c>
     </row>
     <row r="382">
@@ -6297,15 +6273,15 @@
         <v>656</v>
       </c>
       <c r="B382" t="s">
-        <v>239</v>
+        <v>657</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B383" t="s">
-        <v>658</v>
+        <v>302</v>
       </c>
     </row>
     <row r="384">
@@ -6321,7 +6297,7 @@
         <v>661</v>
       </c>
       <c r="B385" t="s">
-        <v>111</v>
+        <v>171</v>
       </c>
     </row>
     <row r="386">
@@ -6329,39 +6305,39 @@
         <v>662</v>
       </c>
       <c r="B386" t="s">
-        <v>663</v>
+        <v>220</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B387" t="s">
-        <v>310</v>
+        <v>521</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="s">
+        <v>664</v>
+      </c>
+      <c r="B388" t="s">
         <v>665</v>
-      </c>
-      <c r="B388" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B389" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
+        <v>667</v>
+      </c>
+      <c r="B390" t="s">
         <v>668</v>
-      </c>
-      <c r="B390" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="391">
@@ -6369,7 +6345,7 @@
         <v>669</v>
       </c>
       <c r="B391" t="s">
-        <v>525</v>
+        <v>153</v>
       </c>
     </row>
     <row r="392">
@@ -6377,15 +6353,15 @@
         <v>670</v>
       </c>
       <c r="B392" t="s">
-        <v>671</v>
+        <v>455</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="s">
+        <v>671</v>
+      </c>
+      <c r="B393" t="s">
         <v>672</v>
-      </c>
-      <c r="B393" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="394">
@@ -6401,63 +6377,63 @@
         <v>675</v>
       </c>
       <c r="B395" t="s">
-        <v>676</v>
+        <v>77</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B396" t="s">
-        <v>153</v>
+        <v>319</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B397" t="s">
-        <v>458</v>
+        <v>34</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="s">
+        <v>678</v>
+      </c>
+      <c r="B398" t="s">
         <v>679</v>
-      </c>
-      <c r="B398" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="s">
+        <v>680</v>
+      </c>
+      <c r="B399" t="s">
         <v>681</v>
-      </c>
-      <c r="B399" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B400" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B401" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="s">
+        <v>684</v>
+      </c>
+      <c r="B402" t="s">
         <v>685</v>
-      </c>
-      <c r="B402" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="403">
@@ -6473,15 +6449,15 @@
         <v>688</v>
       </c>
       <c r="B404" t="s">
-        <v>689</v>
+        <v>298</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="s">
+        <v>689</v>
+      </c>
+      <c r="B405" t="s">
         <v>690</v>
-      </c>
-      <c r="B405" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="406">
@@ -6489,7 +6465,7 @@
         <v>691</v>
       </c>
       <c r="B406" t="s">
-        <v>339</v>
+        <v>687</v>
       </c>
     </row>
     <row r="407">
@@ -6505,15 +6481,15 @@
         <v>694</v>
       </c>
       <c r="B408" t="s">
-        <v>695</v>
+        <v>470</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="s">
+        <v>695</v>
+      </c>
+      <c r="B409" t="s">
         <v>696</v>
-      </c>
-      <c r="B409" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="410">
@@ -6521,55 +6497,55 @@
         <v>697</v>
       </c>
       <c r="B410" t="s">
-        <v>698</v>
+        <v>90</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B411" t="s">
-        <v>695</v>
+        <v>308</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="s">
+        <v>699</v>
+      </c>
+      <c r="B412" t="s">
         <v>700</v>
-      </c>
-      <c r="B412" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B413" t="s">
-        <v>475</v>
+        <v>103</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B414" t="s">
-        <v>704</v>
+        <v>129</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B415" t="s">
-        <v>88</v>
+        <v>704</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="s">
+        <v>705</v>
+      </c>
+      <c r="B416" t="s">
         <v>706</v>
-      </c>
-      <c r="B416" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="417">
@@ -6577,23 +6553,23 @@
         <v>707</v>
       </c>
       <c r="B417" t="s">
-        <v>708</v>
+        <v>119</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B418" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
+        <v>709</v>
+      </c>
+      <c r="B419" t="s">
         <v>710</v>
-      </c>
-      <c r="B419" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="420">
@@ -6601,23 +6577,23 @@
         <v>711</v>
       </c>
       <c r="B420" t="s">
-        <v>712</v>
+        <v>681</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
+        <v>712</v>
+      </c>
+      <c r="B421" t="s">
         <v>713</v>
-      </c>
-      <c r="B421" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
+        <v>714</v>
+      </c>
+      <c r="B422" t="s">
         <v>715</v>
-      </c>
-      <c r="B422" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="423">
@@ -6625,263 +6601,223 @@
         <v>716</v>
       </c>
       <c r="B423" t="s">
-        <v>111</v>
+        <v>717</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>717</v>
+        <v>95</v>
       </c>
       <c r="B424" t="s">
-        <v>718</v>
+        <v>96</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="s">
-        <v>719</v>
+        <v>106</v>
       </c>
       <c r="B425" t="s">
-        <v>689</v>
+        <v>718</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="s">
+        <v>719</v>
+      </c>
+      <c r="B426" t="s">
         <v>720</v>
-      </c>
-      <c r="B426" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B427" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B428" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="s">
-        <v>93</v>
+        <v>214</v>
       </c>
       <c r="B429" t="s">
-        <v>94</v>
+        <v>215</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
-        <v>104</v>
+        <v>723</v>
       </c>
       <c r="B430" t="s">
-        <v>726</v>
+        <v>715</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B431" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="B432" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B433" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
-        <v>214</v>
+        <v>360</v>
       </c>
       <c r="B434" t="s">
-        <v>215</v>
+        <v>361</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
-        <v>731</v>
+        <v>399</v>
       </c>
       <c r="B435" t="s">
-        <v>723</v>
+        <v>400</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
-        <v>732</v>
+        <v>401</v>
       </c>
       <c r="B436" t="s">
-        <v>723</v>
+        <v>402</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="B437" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
-        <v>734</v>
+        <v>412</v>
       </c>
       <c r="B438" t="s">
-        <v>735</v>
+        <v>413</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
-        <v>367</v>
+        <v>432</v>
       </c>
       <c r="B439" t="s">
-        <v>368</v>
+        <v>729</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
-        <v>406</v>
+        <v>436</v>
       </c>
       <c r="B440" t="s">
-        <v>407</v>
+        <v>437</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
-        <v>408</v>
+        <v>730</v>
       </c>
       <c r="B441" t="s">
-        <v>409</v>
+        <v>715</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
-        <v>736</v>
+        <v>574</v>
       </c>
       <c r="B442" t="s">
-        <v>723</v>
+        <v>575</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
-        <v>417</v>
+        <v>628</v>
       </c>
       <c r="B443" t="s">
-        <v>418</v>
+        <v>629</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
-        <v>435</v>
+        <v>731</v>
       </c>
       <c r="B444" t="s">
-        <v>737</v>
+        <v>715</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
-        <v>439</v>
+        <v>732</v>
       </c>
       <c r="B445" t="s">
-        <v>440</v>
+        <v>715</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="B446" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
-        <v>578</v>
+        <v>644</v>
       </c>
       <c r="B447" t="s">
-        <v>579</v>
+        <v>645</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
-        <v>633</v>
+        <v>734</v>
       </c>
       <c r="B448" t="s">
-        <v>634</v>
+        <v>715</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="B449" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B450" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" t="s">
-        <v>741</v>
-      </c>
-      <c r="B451" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" t="s">
-        <v>650</v>
-      </c>
-      <c r="B452" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" t="s">
-        <v>742</v>
-      </c>
-      <c r="B453" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" t="s">
-        <v>743</v>
-      </c>
-      <c r="B454" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" t="s">
-        <v>744</v>
-      </c>
-      <c r="B455" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -6900,7 +6836,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6908,31 +6844,31 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="B2" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B3" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="B4" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
@@ -6940,319 +6876,319 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="B6" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="B7" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="B9" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="B10" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="B11" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="B12" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="B13" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="B14" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="B15" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B16" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="B17" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="B19" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B21" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="B22" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B23" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="B25" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="B26" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="B27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B28" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="B29" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="B31" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="B32" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="B35" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="B36" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="B37" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="B38" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="B39" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B40" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="B41" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B42" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B44" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="B45" t="s">
         <v>224</v>
@@ -7260,119 +7196,119 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="B46" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="B47" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="B48" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="B49" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B50" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="B51" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="B52" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="B53" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="B54" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="B55" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="B56" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="B57" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="B58" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="B59" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="B60" t="s">
         <v>32</v>
@@ -7380,143 +7316,143 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="B61" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="B62" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
       <c r="B63" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
       <c r="B64" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="B65" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="B66" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="B67" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="B68" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="B69" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="B70" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="B71" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="B73" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B74" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="B75" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="B76" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="B77" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="B78" t="s">
         <v>171</v>
@@ -7524,47 +7460,47 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="B79" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="B80" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="B81" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="B82" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="B83" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="B84" t="s">
         <v>220</v>
@@ -7572,23 +7508,23 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="B85" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="B86" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="B87" t="s">
         <v>17</v>
@@ -7596,10 +7532,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -7618,68 +7554,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="B2" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="C2" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="B3" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C3" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="B4" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="C4" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="B5" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="C5" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="B6" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="C6" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>
@@ -7698,332 +7634,332 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="B3" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="C3" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="B4" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="C4" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="B5" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="C5" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="B6" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="C6" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B8" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C8" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="B9" t="s">
         <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="B10" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="C10" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="B11" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="C11" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="B13" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="C13" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="B14" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="C14" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="B15" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="C15" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="B16" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="C16" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="B17" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="C17" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="B20" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="C20" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="B21" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="C21" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="B22" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="C22" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="B24" t="s">
         <v>222</v>
       </c>
       <c r="C24" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="B25" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C25" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="B26" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="C26" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="B27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C27" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="B28" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="C28" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="B29" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="C29" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>964</v>
+        <v>956</v>
       </c>
       <c r="B30" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="C30" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>